<commit_message>
added general stats and subperiod stats to backtesting pdf. worldAnalysis.xlsx -> upload the excel to drive and tickers list also uploaded to drive.
</commit_message>
<xml_diff>
--- a/backtesting/bought_stats.xlsx
+++ b/backtesting/bought_stats.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U41"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,33 +472,30 @@
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Estrategia</t>
         </is>
       </c>
+      <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="n"/>
       <c r="K1" s="1" t="n"/>
-      <c r="L1" s="1" t="n"/>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>S&amp;P-500</t>
+        </is>
+      </c>
       <c r="M1" s="1" t="n"/>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>S&amp;P-500</t>
-        </is>
-      </c>
+      <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="n"/>
       <c r="P1" s="1" t="n"/>
-      <c r="Q1" s="1" t="n"/>
-      <c r="R1" s="1" t="n"/>
-      <c r="S1" s="1" t="n"/>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>q days</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>position</t>
         </is>
@@ -533,71 +530,56 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>%30d</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
+          <t>%60d</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>%90d</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>%180d</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>%total</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
           <t>%30d</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>%60d</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="N2" s="1" t="inlineStr">
         <is>
           <t>%90d</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
+      <c r="O2" s="1" t="inlineStr">
         <is>
           <t>%180d</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="P2" s="1" t="inlineStr">
         <is>
           <t>%total</t>
         </is>
       </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="N2" s="1" t="inlineStr">
-        <is>
-          <t>%30d</t>
-        </is>
-      </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>%60d</t>
-        </is>
-      </c>
-      <c r="P2" s="1" t="inlineStr">
-        <is>
-          <t>%90d</t>
-        </is>
-      </c>
-      <c r="Q2" s="1" t="inlineStr">
-        <is>
-          <t>%180d</t>
-        </is>
-      </c>
-      <c r="R2" s="1" t="inlineStr">
-        <is>
-          <t>%total</t>
-        </is>
-      </c>
-      <c r="S2" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="T2" s="1" t="inlineStr"/>
-      <c r="U2" s="1" t="inlineStr"/>
+      <c r="Q2" s="1" t="inlineStr"/>
+      <c r="R2" s="1" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -613,37 +595,41 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.03049797698319087</v>
+        <v>0.03049755608943399</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03049797698319087</v>
+        <v>0.03049755608943399</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03049797698319087</v>
+        <v>0.03049755608943399</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03049797698319087</v>
+        <v>0.03049755608943399</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03049797698319087</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
+        <v>0.03049755608943399</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0304975560894338</v>
+      </c>
       <c r="H4" t="n">
-        <v>0.03049797698319106</v>
+        <v>0.0304975560894338</v>
       </c>
       <c r="I4" t="n">
-        <v>0.03049797698319106</v>
+        <v>0.0304975560894338</v>
       </c>
       <c r="J4" t="n">
-        <v>0.03049797698319106</v>
+        <v>0.0304975560894338</v>
       </c>
       <c r="K4" t="n">
-        <v>0.03049797698319106</v>
+        <v>0.0304975560894338</v>
       </c>
       <c r="L4" t="n">
-        <v>0.03049797698319106</v>
-      </c>
-      <c r="M4" t="inlineStr"/>
+        <v>-0.009923746383622371</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-0.009923746383622371</v>
+      </c>
       <c r="N4" t="n">
         <v>-0.009923746383622371</v>
       </c>
@@ -654,16 +640,9 @@
         <v>-0.009923746383622371</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.009923746383622371</v>
+        <v>29</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.009923746383622371</v>
-      </c>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="n">
-        <v>29</v>
-      </c>
-      <c r="U4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -674,37 +653,41 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.02382011741111668</v>
+        <v>-0.02382040548061544</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.02382011741111668</v>
+        <v>-0.02382040548061544</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.02382011741111668</v>
+        <v>-0.02382040548061544</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.02382011741111668</v>
+        <v>-0.02382040548061544</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.02382011741111668</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
+        <v>-0.02382040548061544</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-0.02382040548061547</v>
+      </c>
       <c r="H5" t="n">
-        <v>-0.02382011741111684</v>
+        <v>-0.02382040548061547</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.02382011741111684</v>
+        <v>-0.02382040548061547</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.02382011741111684</v>
+        <v>-0.02382040548061547</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.02382011741111684</v>
+        <v>-0.02382040548061547</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.02382011741111684</v>
-      </c>
-      <c r="M5" t="inlineStr"/>
+        <v>0.0009176441131014307</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.0009176441131014307</v>
+      </c>
       <c r="N5" t="n">
         <v>0.0009176441131014307</v>
       </c>
@@ -715,16 +698,9 @@
         <v>0.0009176441131014307</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0009176441131014307</v>
+        <v>16</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0009176441131014307</v>
-      </c>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="n">
-        <v>16</v>
-      </c>
-      <c r="U5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -741,7 +717,7 @@
         <v>0.281260510237367</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4449450058849791</v>
+        <v>0.4449448852726084</v>
       </c>
       <c r="E6" t="n">
         <v>0.435398416130409</v>
@@ -749,43 +725,40 @@
       <c r="F6" t="n">
         <v>0.435398416130409</v>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>0.1707976705167948</v>
+      </c>
       <c r="H6" t="n">
-        <v>0.1707976705167945</v>
+        <v>0.2812605102373671</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2812605102373667</v>
+        <v>0.4449448852726087</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4449450058849785</v>
+        <v>0.4353984161304095</v>
       </c>
       <c r="K6" t="n">
-        <v>0.4353984161304086</v>
+        <v>0.4353984161304095</v>
       </c>
       <c r="L6" t="n">
-        <v>0.4353984161304086</v>
-      </c>
-      <c r="M6" t="inlineStr"/>
+        <v>0.08339445088439368</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.2009919633289186</v>
+      </c>
       <c r="N6" t="n">
-        <v>0.08339445088439368</v>
+        <v>0.1956486874116573</v>
       </c>
       <c r="O6" t="n">
-        <v>0.2009919633289186</v>
+        <v>0.2166834068625899</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1956486874116573</v>
+        <v>0.2166834068625899</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.2166834068625899</v>
+        <v>107</v>
       </c>
       <c r="R6" t="n">
-        <v>0.2166834068625899</v>
-      </c>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="n">
-        <v>107</v>
-      </c>
-      <c r="U6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -810,7 +783,9 @@
       <c r="F7" t="n">
         <v>0</v>
       </c>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
@@ -826,7 +801,9 @@
       <c r="L7" t="n">
         <v>0</v>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
@@ -840,13 +817,6 @@
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -857,39 +827,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.299849614961746</v>
+        <v>0.2998496960668254</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1750016464331122</v>
+        <v>0.175001808643271</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1750016464331122</v>
+        <v>0.175001808643271</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1750016464331122</v>
+        <v>0.175001808643271</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1750016464331122</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
+        <v>0.175001808643271</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.2998496960668245</v>
+      </c>
       <c r="H8" t="n">
-        <v>0.2998496149617456</v>
+        <v>0.1750018086432703</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1750016464331118</v>
+        <v>0.1750018086432703</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1750016464331118</v>
+        <v>0.1750018086432703</v>
       </c>
       <c r="K8" t="n">
-        <v>0.1750016464331118</v>
+        <v>0.1750018086432703</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1750016464331118</v>
-      </c>
-      <c r="M8" t="inlineStr"/>
+        <v>0.08064457782440319</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.02637532821565226</v>
+      </c>
       <c r="N8" t="n">
-        <v>0.08064457782440319</v>
+        <v>0.02637532821565226</v>
       </c>
       <c r="O8" t="n">
         <v>0.02637532821565226</v>
@@ -898,16 +872,9 @@
         <v>0.02637532821565226</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.02637532821565226</v>
+        <v>40</v>
       </c>
       <c r="R8" t="n">
-        <v>0.02637532821565226</v>
-      </c>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="n">
-        <v>40</v>
-      </c>
-      <c r="U8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -918,37 +885,41 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.03228004067161101</v>
+        <v>-0.03228023640420759</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.03228004067161101</v>
+        <v>-0.03228023640420759</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.03228004067161101</v>
+        <v>-0.03228023640420759</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.03228004067161101</v>
+        <v>-0.03228023640420759</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.03228004067161101</v>
-      </c>
-      <c r="G9" t="inlineStr"/>
+        <v>-0.03228023640420759</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-0.03228023640420761</v>
+      </c>
       <c r="H9" t="n">
-        <v>-0.03228004067161103</v>
+        <v>-0.03228023640420761</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.03228004067161103</v>
+        <v>-0.03228023640420761</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.03228004067161103</v>
+        <v>-0.03228023640420761</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.03228004067161103</v>
+        <v>-0.03228023640420761</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.03228004067161103</v>
-      </c>
-      <c r="M9" t="inlineStr"/>
+        <v>-0.009577652178616364</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-0.009577652178616364</v>
+      </c>
       <c r="N9" t="n">
         <v>-0.009577652178616364</v>
       </c>
@@ -959,16 +930,9 @@
         <v>-0.009577652178616364</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.009577652178616364</v>
+        <v>1</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.009577652178616364</v>
-      </c>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="n">
-        <v>1</v>
-      </c>
-      <c r="U9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -979,37 +943,41 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02288800836883258</v>
+        <v>0.02288786758241535</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02288800836883258</v>
+        <v>0.02288786758241535</v>
       </c>
       <c r="D10" t="n">
-        <v>0.02288800836883258</v>
+        <v>0.02288786758241535</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02288800836883258</v>
+        <v>0.02288786758241535</v>
       </c>
       <c r="F10" t="n">
-        <v>0.02288800836883258</v>
-      </c>
-      <c r="G10" t="inlineStr"/>
+        <v>0.02288786758241535</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.02288786758241506</v>
+      </c>
       <c r="H10" t="n">
-        <v>0.02288800836883273</v>
+        <v>0.02288786758241506</v>
       </c>
       <c r="I10" t="n">
-        <v>0.02288800836883273</v>
+        <v>0.02288786758241506</v>
       </c>
       <c r="J10" t="n">
-        <v>0.02288800836883273</v>
+        <v>0.02288786758241506</v>
       </c>
       <c r="K10" t="n">
-        <v>0.02288800836883273</v>
+        <v>0.02288786758241506</v>
       </c>
       <c r="L10" t="n">
-        <v>0.02288800836883273</v>
-      </c>
-      <c r="M10" t="inlineStr"/>
+        <v>0.02752777333261759</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.02752777333261759</v>
+      </c>
       <c r="N10" t="n">
         <v>0.02752777333261759</v>
       </c>
@@ -1020,16 +988,9 @@
         <v>0.02752777333261759</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.02752777333261759</v>
+        <v>16</v>
       </c>
       <c r="R10" t="n">
-        <v>0.02752777333261759</v>
-      </c>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="n">
-        <v>16</v>
-      </c>
-      <c r="U10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1040,37 +1001,41 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.0407783947466876</v>
+        <v>-0.04077852574414415</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0407783947466876</v>
+        <v>-0.04077852574414415</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.0407783947466876</v>
+        <v>-0.04077852574414415</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.0407783947466876</v>
+        <v>-0.04077852574414415</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0407783947466876</v>
-      </c>
-      <c r="G11" t="inlineStr"/>
+        <v>-0.04077852574414415</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.04077852574414399</v>
+      </c>
       <c r="H11" t="n">
-        <v>-0.04077839474668738</v>
+        <v>-0.04077852574414399</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.04077839474668738</v>
+        <v>-0.04077852574414399</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.04077839474668738</v>
+        <v>-0.04077852574414399</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.04077839474668738</v>
+        <v>-0.04077852574414399</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.04077839474668738</v>
-      </c>
-      <c r="M11" t="inlineStr"/>
+        <v>0.01941909467670414</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.01941909467670414</v>
+      </c>
       <c r="N11" t="n">
         <v>0.01941909467670414</v>
       </c>
@@ -1081,16 +1046,9 @@
         <v>0.01941909467670414</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.01941909467670414</v>
+        <v>17</v>
       </c>
       <c r="R11" t="n">
-        <v>0.01941909467670414</v>
-      </c>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="n">
-        <v>17</v>
-      </c>
-      <c r="U11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1101,39 +1059,43 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.1232255604576767</v>
+        <v>0.1232256910590129</v>
       </c>
       <c r="C12" t="n">
-        <v>0.06341876815644264</v>
+        <v>0.06341889875777885</v>
       </c>
       <c r="D12" t="n">
-        <v>0.06341876815644264</v>
+        <v>0.06341889875777885</v>
       </c>
       <c r="E12" t="n">
-        <v>0.06341876815644264</v>
+        <v>0.06341889875777885</v>
       </c>
       <c r="F12" t="n">
-        <v>0.06341876815644264</v>
-      </c>
-      <c r="G12" t="inlineStr"/>
+        <v>0.06341889875777885</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1232256910590126</v>
+      </c>
       <c r="H12" t="n">
-        <v>0.1232255604576767</v>
+        <v>0.06341889875777876</v>
       </c>
       <c r="I12" t="n">
-        <v>0.06341876815644254</v>
+        <v>0.06341889875777876</v>
       </c>
       <c r="J12" t="n">
-        <v>0.06341876815644254</v>
+        <v>0.06341889875777876</v>
       </c>
       <c r="K12" t="n">
-        <v>0.06341876815644254</v>
+        <v>0.06341889875777876</v>
       </c>
       <c r="L12" t="n">
-        <v>0.06341876815644254</v>
-      </c>
-      <c r="M12" t="inlineStr"/>
+        <v>0.03048631688566067</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.0349317886860872</v>
+      </c>
       <c r="N12" t="n">
-        <v>0.03048631688566067</v>
+        <v>0.0349317886860872</v>
       </c>
       <c r="O12" t="n">
         <v>0.0349317886860872</v>
@@ -1142,16 +1104,9 @@
         <v>0.0349317886860872</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.0349317886860872</v>
+        <v>37</v>
       </c>
       <c r="R12" t="n">
-        <v>0.0349317886860872</v>
-      </c>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="n">
-        <v>37</v>
-      </c>
-      <c r="U12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1162,37 +1117,41 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.02324883830870228</v>
+        <v>-0.02324883557129243</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.02324883830870228</v>
+        <v>-0.02324883557129243</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.02324883830870228</v>
+        <v>-0.02324883557129243</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.02324883830870228</v>
+        <v>-0.02324883557129243</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.02324883830870228</v>
-      </c>
-      <c r="G13" t="inlineStr"/>
+        <v>-0.02324883557129243</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-0.02324883557129245</v>
+      </c>
       <c r="H13" t="n">
-        <v>-0.02324883830870228</v>
+        <v>-0.02324883557129245</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.02324883830870228</v>
+        <v>-0.02324883557129245</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.02324883830870228</v>
+        <v>-0.02324883557129245</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.02324883830870228</v>
+        <v>-0.02324883557129245</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.02324883830870228</v>
-      </c>
-      <c r="M13" t="inlineStr"/>
+        <v>-0.006554750898592477</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-0.006554750898592477</v>
+      </c>
       <c r="N13" t="n">
         <v>-0.006554750898592477</v>
       </c>
@@ -1203,16 +1162,9 @@
         <v>-0.006554750898592477</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.006554750898592477</v>
+        <v>3</v>
       </c>
       <c r="R13" t="n">
-        <v>-0.006554750898592477</v>
-      </c>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="n">
-        <v>3</v>
-      </c>
-      <c r="U13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1237,7 +1189,9 @@
       <c r="F14" t="n">
         <v>0</v>
       </c>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
       <c r="H14" t="n">
         <v>0</v>
       </c>
@@ -1253,7 +1207,9 @@
       <c r="L14" t="n">
         <v>0</v>
       </c>
-      <c r="M14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
@@ -1267,13 +1223,6 @@
         <v>0</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="n">
-        <v>0</v>
-      </c>
-      <c r="U14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1284,37 +1233,41 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.03587339925545947</v>
+        <v>-0.03587341148084575</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.03587339925545947</v>
+        <v>-0.03587341148084575</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.03587339925545947</v>
+        <v>-0.03587341148084575</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.03587339925545947</v>
+        <v>-0.03587341148084575</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.03587339925545947</v>
-      </c>
-      <c r="G15" t="inlineStr"/>
+        <v>-0.03587341148084575</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-0.03587341148084562</v>
+      </c>
       <c r="H15" t="n">
-        <v>-0.03587339925545923</v>
+        <v>-0.03587341148084562</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.03587339925545923</v>
+        <v>-0.03587341148084562</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.03587339925545923</v>
+        <v>-0.03587341148084562</v>
       </c>
       <c r="K15" t="n">
-        <v>-0.03587339925545923</v>
+        <v>-0.03587341148084562</v>
       </c>
       <c r="L15" t="n">
-        <v>-0.03587339925545923</v>
-      </c>
-      <c r="M15" t="inlineStr"/>
+        <v>-0.03603102867633897</v>
+      </c>
+      <c r="M15" t="n">
+        <v>-0.03603102867633897</v>
+      </c>
       <c r="N15" t="n">
         <v>-0.03603102867633897</v>
       </c>
@@ -1325,16 +1278,9 @@
         <v>-0.03603102867633897</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.03603102867633897</v>
+        <v>8</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.03603102867633897</v>
-      </c>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="n">
-        <v>8</v>
-      </c>
-      <c r="U15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1359,23 +1305,27 @@
       <c r="F16" t="n">
         <v>0.002533028598966356</v>
       </c>
-      <c r="G16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>0.002533028598966393</v>
+      </c>
       <c r="H16" t="n">
-        <v>0.002533028598966498</v>
+        <v>0.002533028598966393</v>
       </c>
       <c r="I16" t="n">
-        <v>0.002533028598966498</v>
+        <v>0.002533028598966393</v>
       </c>
       <c r="J16" t="n">
-        <v>0.002533028598966498</v>
+        <v>0.002533028598966393</v>
       </c>
       <c r="K16" t="n">
-        <v>0.002533028598966498</v>
+        <v>0.002533028598966393</v>
       </c>
       <c r="L16" t="n">
-        <v>0.002533028598966498</v>
-      </c>
-      <c r="M16" t="inlineStr"/>
+        <v>0.02353960417202901</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.02353960417202901</v>
+      </c>
       <c r="N16" t="n">
         <v>0.02353960417202901</v>
       </c>
@@ -1386,16 +1336,9 @@
         <v>0.02353960417202901</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.02353960417202901</v>
+        <v>9</v>
       </c>
       <c r="R16" t="n">
-        <v>0.02353960417202901</v>
-      </c>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="n">
-        <v>9</v>
-      </c>
-      <c r="U16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1406,37 +1349,41 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.03390519663200985</v>
+        <v>-0.0339049519749999</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.03390519663200985</v>
+        <v>-0.0339049519749999</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.03390519663200985</v>
+        <v>-0.0339049519749999</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.03390519663200985</v>
+        <v>-0.0339049519749999</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.03390519663200985</v>
-      </c>
-      <c r="G17" t="inlineStr"/>
+        <v>-0.0339049519749999</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-0.03390495197499985</v>
+      </c>
       <c r="H17" t="n">
-        <v>-0.03390519663200986</v>
+        <v>-0.03390495197499985</v>
       </c>
       <c r="I17" t="n">
-        <v>-0.03390519663200986</v>
+        <v>-0.03390495197499985</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.03390519663200986</v>
+        <v>-0.03390495197499985</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.03390519663200986</v>
+        <v>-0.03390495197499985</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.03390519663200986</v>
-      </c>
-      <c r="M17" t="inlineStr"/>
+        <v>-0.01476053931945923</v>
+      </c>
+      <c r="M17" t="n">
+        <v>-0.01476053931945923</v>
+      </c>
       <c r="N17" t="n">
         <v>-0.01476053931945923</v>
       </c>
@@ -1447,16 +1394,9 @@
         <v>-0.01476053931945923</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.01476053931945923</v>
+        <v>1</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.01476053931945923</v>
-      </c>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="n">
-        <v>1</v>
-      </c>
-      <c r="U17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1467,37 +1407,41 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.01999345760339495</v>
+        <v>-0.01999339679019644</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.01999345760339495</v>
+        <v>-0.01999339679019644</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.01999345760339495</v>
+        <v>-0.01999339679019644</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.01999345760339495</v>
+        <v>-0.01999339679019644</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.01999345760339495</v>
-      </c>
-      <c r="G18" t="inlineStr"/>
+        <v>-0.01999339679019644</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-0.01999339679019641</v>
+      </c>
       <c r="H18" t="n">
-        <v>-0.01999345760339495</v>
+        <v>-0.01999339679019641</v>
       </c>
       <c r="I18" t="n">
-        <v>-0.01999345760339495</v>
+        <v>-0.01999339679019641</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.01999345760339495</v>
+        <v>-0.01999339679019641</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.01999345760339495</v>
+        <v>-0.01999339679019641</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.01999345760339495</v>
-      </c>
-      <c r="M18" t="inlineStr"/>
+        <v>-0.005467336018314979</v>
+      </c>
+      <c r="M18" t="n">
+        <v>-0.005467336018314979</v>
+      </c>
       <c r="N18" t="n">
         <v>-0.005467336018314979</v>
       </c>
@@ -1508,16 +1452,9 @@
         <v>-0.005467336018314979</v>
       </c>
       <c r="Q18" t="n">
-        <v>-0.005467336018314979</v>
+        <v>1</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.005467336018314979</v>
-      </c>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="n">
-        <v>1</v>
-      </c>
-      <c r="U18" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1528,37 +1465,41 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.0687806853216088</v>
+        <v>0.06878023921580383</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0687806853216088</v>
+        <v>0.06878023921580383</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0687806853216088</v>
+        <v>0.06878023921580383</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0687806853216088</v>
+        <v>0.06878023921580383</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0687806853216088</v>
-      </c>
-      <c r="G19" t="inlineStr"/>
+        <v>0.06878023921580383</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.06878023921580402</v>
+      </c>
       <c r="H19" t="n">
-        <v>0.06878068532160921</v>
+        <v>0.06878023921580402</v>
       </c>
       <c r="I19" t="n">
-        <v>0.06878068532160921</v>
+        <v>0.06878023921580402</v>
       </c>
       <c r="J19" t="n">
-        <v>0.06878068532160921</v>
+        <v>0.06878023921580402</v>
       </c>
       <c r="K19" t="n">
-        <v>0.06878068532160921</v>
+        <v>0.06878023921580402</v>
       </c>
       <c r="L19" t="n">
-        <v>0.06878068532160921</v>
-      </c>
-      <c r="M19" t="inlineStr"/>
+        <v>0.04012562594941583</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.04012562594941583</v>
+      </c>
       <c r="N19" t="n">
         <v>0.04012562594941583</v>
       </c>
@@ -1569,16 +1510,9 @@
         <v>0.04012562594941583</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.04012562594941583</v>
+        <v>29</v>
       </c>
       <c r="R19" t="n">
-        <v>0.04012562594941583</v>
-      </c>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="n">
-        <v>29</v>
-      </c>
-      <c r="U19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1589,39 +1523,43 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1482922620374998</v>
+        <v>0.1482923144610329</v>
       </c>
       <c r="C20" t="n">
-        <v>0.15583805589171</v>
+        <v>0.1558381078507913</v>
       </c>
       <c r="D20" t="n">
-        <v>0.15583805589171</v>
+        <v>0.1558381078507913</v>
       </c>
       <c r="E20" t="n">
-        <v>0.15583805589171</v>
+        <v>0.1558381078507913</v>
       </c>
       <c r="F20" t="n">
-        <v>0.15583805589171</v>
-      </c>
-      <c r="G20" t="inlineStr"/>
+        <v>0.1558381078507913</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1482923144610336</v>
+      </c>
       <c r="H20" t="n">
-        <v>0.1482922620374998</v>
+        <v>0.1558381078507921</v>
       </c>
       <c r="I20" t="n">
-        <v>0.15583805589171</v>
+        <v>0.1558381078507921</v>
       </c>
       <c r="J20" t="n">
-        <v>0.15583805589171</v>
+        <v>0.1558381078507921</v>
       </c>
       <c r="K20" t="n">
-        <v>0.15583805589171</v>
+        <v>0.1558381078507921</v>
       </c>
       <c r="L20" t="n">
-        <v>0.15583805589171</v>
-      </c>
-      <c r="M20" t="inlineStr"/>
+        <v>0.03113906066292487</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.03800766019713923</v>
+      </c>
       <c r="N20" t="n">
-        <v>0.03113906066292487</v>
+        <v>0.03800766019713923</v>
       </c>
       <c r="O20" t="n">
         <v>0.03800766019713923</v>
@@ -1630,16 +1568,9 @@
         <v>0.03800766019713923</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.03800766019713923</v>
+        <v>56</v>
       </c>
       <c r="R20" t="n">
-        <v>0.03800766019713923</v>
-      </c>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="n">
-        <v>56</v>
-      </c>
-      <c r="U20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1650,37 +1581,41 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.00402213821322395</v>
+        <v>-0.004021717188442952</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.00402213821322395</v>
+        <v>-0.004021717188442952</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.00402213821322395</v>
+        <v>-0.004021717188442952</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.00402213821322395</v>
+        <v>-0.004021717188442952</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.00402213821322395</v>
-      </c>
-      <c r="G21" t="inlineStr"/>
+        <v>-0.004021717188442952</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-0.004021717188442946</v>
+      </c>
       <c r="H21" t="n">
-        <v>-0.0040221382132239</v>
+        <v>-0.004021717188442946</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.0040221382132239</v>
+        <v>-0.004021717188442946</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.0040221382132239</v>
+        <v>-0.004021717188442946</v>
       </c>
       <c r="K21" t="n">
-        <v>-0.0040221382132239</v>
+        <v>-0.004021717188442946</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.0040221382132239</v>
-      </c>
-      <c r="M21" t="inlineStr"/>
+        <v>0.007690773777572331</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.007690773777572331</v>
+      </c>
       <c r="N21" t="n">
         <v>0.007690773777572331</v>
       </c>
@@ -1691,16 +1626,9 @@
         <v>0.007690773777572331</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.007690773777572331</v>
+        <v>2</v>
       </c>
       <c r="R21" t="n">
-        <v>0.007690773777572331</v>
-      </c>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="n">
-        <v>2</v>
-      </c>
-      <c r="U21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1711,37 +1639,41 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.01837677908476055</v>
+        <v>-0.01837698476126817</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.01837677908476055</v>
+        <v>-0.01837698476126817</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.01837677908476055</v>
+        <v>-0.01837698476126817</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.01837677908476055</v>
+        <v>-0.01837698476126817</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.01837677908476055</v>
-      </c>
-      <c r="G22" t="inlineStr"/>
+        <v>-0.01837698476126817</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-0.01837698476126834</v>
+      </c>
       <c r="H22" t="n">
-        <v>-0.0183767790847607</v>
+        <v>-0.01837698476126834</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.0183767790847607</v>
+        <v>-0.01837698476126834</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.0183767790847607</v>
+        <v>-0.01837698476126834</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.0183767790847607</v>
+        <v>-0.01837698476126834</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.0183767790847607</v>
-      </c>
-      <c r="M22" t="inlineStr"/>
+        <v>-0.01515890341735676</v>
+      </c>
+      <c r="M22" t="n">
+        <v>-0.01515890341735676</v>
+      </c>
       <c r="N22" t="n">
         <v>-0.01515890341735676</v>
       </c>
@@ -1752,16 +1684,9 @@
         <v>-0.01515890341735676</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.01515890341735676</v>
+        <v>5</v>
       </c>
       <c r="R22" t="n">
-        <v>-0.01515890341735676</v>
-      </c>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="n">
-        <v>5</v>
-      </c>
-      <c r="U22" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1786,23 +1711,27 @@
       <c r="F23" t="n">
         <v>-0.01449492137648673</v>
       </c>
-      <c r="G23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>-0.01449492137648672</v>
+      </c>
       <c r="H23" t="n">
-        <v>-0.01449492137648673</v>
+        <v>-0.01449492137648672</v>
       </c>
       <c r="I23" t="n">
-        <v>-0.01449492137648673</v>
+        <v>-0.01449492137648672</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.01449492137648673</v>
+        <v>-0.01449492137648672</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.01449492137648673</v>
+        <v>-0.01449492137648672</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.01449492137648673</v>
-      </c>
-      <c r="M23" t="inlineStr"/>
+        <v>-0.002127407476523251</v>
+      </c>
+      <c r="M23" t="n">
+        <v>-0.002127407476523251</v>
+      </c>
       <c r="N23" t="n">
         <v>-0.002127407476523251</v>
       </c>
@@ -1813,16 +1742,9 @@
         <v>-0.002127407476523251</v>
       </c>
       <c r="Q23" t="n">
-        <v>-0.002127407476523251</v>
+        <v>3</v>
       </c>
       <c r="R23" t="n">
-        <v>-0.002127407476523251</v>
-      </c>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="n">
-        <v>3</v>
-      </c>
-      <c r="U23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1833,37 +1755,41 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.02710273714743404</v>
+        <v>-0.02710283273604424</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.02710273714743404</v>
+        <v>-0.02710283273604424</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.02710273714743404</v>
+        <v>-0.02710283273604424</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.02710273714743404</v>
+        <v>-0.02710283273604424</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.02710273714743404</v>
-      </c>
-      <c r="G24" t="inlineStr"/>
+        <v>-0.02710283273604424</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-0.02710283273604438</v>
+      </c>
       <c r="H24" t="n">
-        <v>-0.02710273714743392</v>
+        <v>-0.02710283273604438</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.02710273714743392</v>
+        <v>-0.02710283273604438</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.02710273714743392</v>
+        <v>-0.02710283273604438</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.02710273714743392</v>
+        <v>-0.02710283273604438</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.02710273714743392</v>
-      </c>
-      <c r="M24" t="inlineStr"/>
+        <v>-0.01550302847601963</v>
+      </c>
+      <c r="M24" t="n">
+        <v>-0.01550302847601963</v>
+      </c>
       <c r="N24" t="n">
         <v>-0.01550302847601963</v>
       </c>
@@ -1874,16 +1800,9 @@
         <v>-0.01550302847601963</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.01550302847601963</v>
+        <v>11</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.01550302847601963</v>
-      </c>
-      <c r="S24" t="inlineStr"/>
-      <c r="T24" t="n">
-        <v>11</v>
-      </c>
-      <c r="U24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1894,37 +1813,41 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.02275512760720923</v>
+        <v>0.02275545300368625</v>
       </c>
       <c r="C25" t="n">
-        <v>0.02275512760720923</v>
+        <v>0.02275545300368625</v>
       </c>
       <c r="D25" t="n">
-        <v>0.02275512760720923</v>
+        <v>0.02275545300368625</v>
       </c>
       <c r="E25" t="n">
-        <v>0.02275512760720923</v>
+        <v>0.02275545300368625</v>
       </c>
       <c r="F25" t="n">
-        <v>0.02275512760720923</v>
-      </c>
-      <c r="G25" t="inlineStr"/>
+        <v>0.02275545300368625</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.02275545300368611</v>
+      </c>
       <c r="H25" t="n">
-        <v>0.02275512760720942</v>
+        <v>0.02275545300368611</v>
       </c>
       <c r="I25" t="n">
-        <v>0.02275512760720942</v>
+        <v>0.02275545300368611</v>
       </c>
       <c r="J25" t="n">
-        <v>0.02275512760720942</v>
+        <v>0.02275545300368611</v>
       </c>
       <c r="K25" t="n">
-        <v>0.02275512760720942</v>
+        <v>0.02275545300368611</v>
       </c>
       <c r="L25" t="n">
-        <v>0.02275512760720942</v>
-      </c>
-      <c r="M25" t="inlineStr"/>
+        <v>0.03921389622299688</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.03921389622299688</v>
+      </c>
       <c r="N25" t="n">
         <v>0.03921389622299688</v>
       </c>
@@ -1935,16 +1858,9 @@
         <v>0.03921389622299688</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.03921389622299688</v>
+        <v>26</v>
       </c>
       <c r="R25" t="n">
-        <v>0.03921389622299688</v>
-      </c>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="n">
-        <v>26</v>
-      </c>
-      <c r="U25" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1955,39 +1871,43 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.195333061913076</v>
+        <v>0.1953335142344227</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1661332008648636</v>
+        <v>0.1661332350945641</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1661332008648636</v>
+        <v>0.1661332350945641</v>
       </c>
       <c r="E26" t="n">
-        <v>0.1661332008648636</v>
+        <v>0.1661332350945641</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1661332008648636</v>
-      </c>
-      <c r="G26" t="inlineStr"/>
+        <v>0.1661332350945641</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.1953335142344226</v>
+      </c>
       <c r="H26" t="n">
-        <v>0.1953330619130765</v>
+        <v>0.1661332350945638</v>
       </c>
       <c r="I26" t="n">
-        <v>0.1661332008648635</v>
+        <v>0.1661332350945638</v>
       </c>
       <c r="J26" t="n">
-        <v>0.1661332008648635</v>
+        <v>0.1661332350945638</v>
       </c>
       <c r="K26" t="n">
-        <v>0.1661332008648635</v>
+        <v>0.1661332350945638</v>
       </c>
       <c r="L26" t="n">
-        <v>0.1661332008648635</v>
-      </c>
-      <c r="M26" t="inlineStr"/>
+        <v>0.005776521332744687</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.003796932215573658</v>
+      </c>
       <c r="N26" t="n">
-        <v>0.005776521332744687</v>
+        <v>0.003796932215573658</v>
       </c>
       <c r="O26" t="n">
         <v>0.003796932215573658</v>
@@ -1996,16 +1916,9 @@
         <v>0.003796932215573658</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.003796932215573658</v>
+        <v>51</v>
       </c>
       <c r="R26" t="n">
-        <v>0.003796932215573658</v>
-      </c>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="n">
-        <v>51</v>
-      </c>
-      <c r="U26" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2016,37 +1929,41 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.03390064128606267</v>
+        <v>-0.03390054987580626</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.03390064128606267</v>
+        <v>-0.03390054987580626</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.03390064128606267</v>
+        <v>-0.03390054987580626</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.03390064128606267</v>
+        <v>-0.03390054987580626</v>
       </c>
       <c r="F27" t="n">
-        <v>-0.03390064128606267</v>
-      </c>
-      <c r="G27" t="inlineStr"/>
+        <v>-0.03390054987580626</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-0.0339005498758063</v>
+      </c>
       <c r="H27" t="n">
-        <v>-0.0339006412860625</v>
+        <v>-0.0339005498758063</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.0339006412860625</v>
+        <v>-0.0339005498758063</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.0339006412860625</v>
+        <v>-0.0339005498758063</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.0339006412860625</v>
+        <v>-0.0339005498758063</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.0339006412860625</v>
-      </c>
-      <c r="M27" t="inlineStr"/>
+        <v>-0.02146132191215122</v>
+      </c>
+      <c r="M27" t="n">
+        <v>-0.02146132191215122</v>
+      </c>
       <c r="N27" t="n">
         <v>-0.02146132191215122</v>
       </c>
@@ -2057,16 +1974,9 @@
         <v>-0.02146132191215122</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.02146132191215122</v>
+        <v>11</v>
       </c>
       <c r="R27" t="n">
-        <v>-0.02146132191215122</v>
-      </c>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="n">
-        <v>11</v>
-      </c>
-      <c r="U27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2077,37 +1987,41 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.0226284896443995</v>
+        <v>-0.0226285769407343</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.0226284896443995</v>
+        <v>-0.0226285769407343</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.0226284896443995</v>
+        <v>-0.0226285769407343</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.0226284896443995</v>
+        <v>-0.0226285769407343</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.0226284896443995</v>
-      </c>
-      <c r="G28" t="inlineStr"/>
+        <v>-0.0226285769407343</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-0.02262857694073438</v>
+      </c>
       <c r="H28" t="n">
-        <v>-0.02262848964439947</v>
+        <v>-0.02262857694073438</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.02262848964439947</v>
+        <v>-0.02262857694073438</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.02262848964439947</v>
+        <v>-0.02262857694073438</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.02262848964439947</v>
+        <v>-0.02262857694073438</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.02262848964439947</v>
-      </c>
-      <c r="M28" t="inlineStr"/>
+        <v>-0.0203105883298563</v>
+      </c>
+      <c r="M28" t="n">
+        <v>-0.0203105883298563</v>
+      </c>
       <c r="N28" t="n">
         <v>-0.0203105883298563</v>
       </c>
@@ -2118,16 +2032,9 @@
         <v>-0.0203105883298563</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.0203105883298563</v>
+        <v>2</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.0203105883298563</v>
-      </c>
-      <c r="S28" t="inlineStr"/>
-      <c r="T28" t="n">
-        <v>2</v>
-      </c>
-      <c r="U28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2138,37 +2045,41 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.002237332707471198</v>
+        <v>0.002237519555082903</v>
       </c>
       <c r="C29" t="n">
-        <v>0.002237332707471198</v>
+        <v>0.002237519555082903</v>
       </c>
       <c r="D29" t="n">
-        <v>0.002237332707471198</v>
+        <v>0.002237519555082903</v>
       </c>
       <c r="E29" t="n">
-        <v>0.002237332707471198</v>
+        <v>0.002237519555082903</v>
       </c>
       <c r="F29" t="n">
-        <v>0.002237332707471198</v>
-      </c>
-      <c r="G29" t="inlineStr"/>
+        <v>0.002237519555082903</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.002237519555082634</v>
+      </c>
       <c r="H29" t="n">
-        <v>0.002237332707471543</v>
+        <v>0.002237519555082634</v>
       </c>
       <c r="I29" t="n">
-        <v>0.002237332707471543</v>
+        <v>0.002237519555082634</v>
       </c>
       <c r="J29" t="n">
-        <v>0.002237332707471543</v>
+        <v>0.002237519555082634</v>
       </c>
       <c r="K29" t="n">
-        <v>0.002237332707471543</v>
+        <v>0.002237519555082634</v>
       </c>
       <c r="L29" t="n">
-        <v>0.002237332707471543</v>
-      </c>
-      <c r="M29" t="inlineStr"/>
+        <v>-0.01090527365137864</v>
+      </c>
+      <c r="M29" t="n">
+        <v>-0.01090527365137864</v>
+      </c>
       <c r="N29" t="n">
         <v>-0.01090527365137864</v>
       </c>
@@ -2179,16 +2090,9 @@
         <v>-0.01090527365137864</v>
       </c>
       <c r="Q29" t="n">
-        <v>-0.01090527365137864</v>
+        <v>21</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.01090527365137864</v>
-      </c>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="n">
-        <v>21</v>
-      </c>
-      <c r="U29" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2213,7 +2117,9 @@
       <c r="F30" t="n">
         <v>0</v>
       </c>
-      <c r="G30" t="inlineStr"/>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
       <c r="H30" t="n">
         <v>0</v>
       </c>
@@ -2229,7 +2135,9 @@
       <c r="L30" t="n">
         <v>0</v>
       </c>
-      <c r="M30" t="inlineStr"/>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
       <c r="N30" t="n">
         <v>0</v>
       </c>
@@ -2243,13 +2151,6 @@
         <v>0</v>
       </c>
       <c r="R30" t="n">
-        <v>0</v>
-      </c>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="n">
-        <v>0</v>
-      </c>
-      <c r="U30" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2260,37 +2161,41 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.01447154100743848</v>
+        <v>0.01447134741529104</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01447154100743848</v>
+        <v>0.01447134741529104</v>
       </c>
       <c r="D31" t="n">
-        <v>0.01447154100743848</v>
+        <v>0.01447134741529104</v>
       </c>
       <c r="E31" t="n">
-        <v>0.01447154100743848</v>
+        <v>0.01447134741529104</v>
       </c>
       <c r="F31" t="n">
-        <v>0.01447154100743848</v>
-      </c>
-      <c r="G31" t="inlineStr"/>
+        <v>0.01447134741529104</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.01447134741529098</v>
+      </c>
       <c r="H31" t="n">
-        <v>0.01447154100743813</v>
+        <v>0.01447134741529098</v>
       </c>
       <c r="I31" t="n">
-        <v>0.01447154100743813</v>
+        <v>0.01447134741529098</v>
       </c>
       <c r="J31" t="n">
-        <v>0.01447154100743813</v>
+        <v>0.01447134741529098</v>
       </c>
       <c r="K31" t="n">
-        <v>0.01447154100743813</v>
+        <v>0.01447134741529098</v>
       </c>
       <c r="L31" t="n">
-        <v>0.01447154100743813</v>
-      </c>
-      <c r="M31" t="inlineStr"/>
+        <v>-0.01480345950908564</v>
+      </c>
+      <c r="M31" t="n">
+        <v>-0.01480345950908564</v>
+      </c>
       <c r="N31" t="n">
         <v>-0.01480345950908564</v>
       </c>
@@ -2301,16 +2206,9 @@
         <v>-0.01480345950908564</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.01480345950908564</v>
+        <v>25</v>
       </c>
       <c r="R31" t="n">
-        <v>-0.01480345950908564</v>
-      </c>
-      <c r="S31" t="inlineStr"/>
-      <c r="T31" t="n">
-        <v>25</v>
-      </c>
-      <c r="U31" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2335,23 +2233,27 @@
       <c r="F32" t="n">
         <v>-0.03749707021509817</v>
       </c>
-      <c r="G32" t="inlineStr"/>
+      <c r="G32" t="n">
+        <v>-0.03749707021509832</v>
+      </c>
       <c r="H32" t="n">
-        <v>-0.03749707021509797</v>
+        <v>-0.03749707021509832</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.03749707021509797</v>
+        <v>-0.03749707021509832</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.03749707021509797</v>
+        <v>-0.03749707021509832</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.03749707021509797</v>
+        <v>-0.03749707021509832</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.03749707021509797</v>
-      </c>
-      <c r="M32" t="inlineStr"/>
+        <v>-0.03363726966771335</v>
+      </c>
+      <c r="M32" t="n">
+        <v>-0.03363726966771335</v>
+      </c>
       <c r="N32" t="n">
         <v>-0.03363726966771335</v>
       </c>
@@ -2362,16 +2264,9 @@
         <v>-0.03363726966771335</v>
       </c>
       <c r="Q32" t="n">
-        <v>-0.03363726966771335</v>
+        <v>18</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.03363726966771335</v>
-      </c>
-      <c r="S32" t="inlineStr"/>
-      <c r="T32" t="n">
-        <v>18</v>
-      </c>
-      <c r="U32" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2396,23 +2291,27 @@
       <c r="F33" t="n">
         <v>-0.0346488060584702</v>
       </c>
-      <c r="G33" t="inlineStr"/>
+      <c r="G33" t="n">
+        <v>-0.03464880605847014</v>
+      </c>
       <c r="H33" t="n">
-        <v>-0.03464880605847024</v>
+        <v>-0.03464880605847014</v>
       </c>
       <c r="I33" t="n">
-        <v>-0.03464880605847024</v>
+        <v>-0.03464880605847014</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.03464880605847024</v>
+        <v>-0.03464880605847014</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.03464880605847024</v>
+        <v>-0.03464880605847014</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.03464880605847024</v>
-      </c>
-      <c r="M33" t="inlineStr"/>
+        <v>-0.04614882783647748</v>
+      </c>
+      <c r="M33" t="n">
+        <v>-0.04614882783647748</v>
+      </c>
       <c r="N33" t="n">
         <v>-0.04614882783647748</v>
       </c>
@@ -2423,16 +2322,9 @@
         <v>-0.04614882783647748</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.04614882783647748</v>
+        <v>4</v>
       </c>
       <c r="R33" t="n">
-        <v>-0.04614882783647748</v>
-      </c>
-      <c r="S33" t="inlineStr"/>
-      <c r="T33" t="n">
-        <v>4</v>
-      </c>
-      <c r="U33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2443,37 +2335,41 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.04921693319140842</v>
+        <v>0.04921703372378769</v>
       </c>
       <c r="C34" t="n">
-        <v>0.04921693319140842</v>
+        <v>0.04921703372378769</v>
       </c>
       <c r="D34" t="n">
-        <v>0.04921693319140842</v>
+        <v>0.04921703372378769</v>
       </c>
       <c r="E34" t="n">
-        <v>0.04921693319140842</v>
+        <v>0.04921703372378769</v>
       </c>
       <c r="F34" t="n">
-        <v>0.04921693319140842</v>
-      </c>
-      <c r="G34" t="inlineStr"/>
+        <v>0.04921703372378769</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.04921703372378691</v>
+      </c>
       <c r="H34" t="n">
-        <v>0.04921693319140805</v>
+        <v>0.04921703372378691</v>
       </c>
       <c r="I34" t="n">
-        <v>0.04921693319140805</v>
+        <v>0.04921703372378691</v>
       </c>
       <c r="J34" t="n">
-        <v>0.04921693319140805</v>
+        <v>0.04921703372378691</v>
       </c>
       <c r="K34" t="n">
-        <v>0.04921693319140805</v>
+        <v>0.04921703372378691</v>
       </c>
       <c r="L34" t="n">
-        <v>0.04921693319140805</v>
-      </c>
-      <c r="M34" t="inlineStr"/>
+        <v>0.04405387465293983</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.04405387465293983</v>
+      </c>
       <c r="N34" t="n">
         <v>0.04405387465293983</v>
       </c>
@@ -2484,16 +2380,9 @@
         <v>0.04405387465293983</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.04405387465293983</v>
+        <v>29</v>
       </c>
       <c r="R34" t="n">
-        <v>0.04405387465293983</v>
-      </c>
-      <c r="S34" t="inlineStr"/>
-      <c r="T34" t="n">
-        <v>29</v>
-      </c>
-      <c r="U34" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2504,37 +2393,41 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.008716198511418777</v>
+        <v>-0.008716199320743526</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.008716198511418777</v>
+        <v>-0.008716199320743526</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.008716198511418777</v>
+        <v>-0.008716199320743526</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.008716198511418777</v>
+        <v>-0.008716199320743526</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.008716198511418777</v>
-      </c>
-      <c r="G35" t="inlineStr"/>
+        <v>-0.008716199320743526</v>
+      </c>
+      <c r="G35" t="n">
+        <v>-0.008716199320743427</v>
+      </c>
       <c r="H35" t="n">
-        <v>-0.008716198511418954</v>
+        <v>-0.008716199320743427</v>
       </c>
       <c r="I35" t="n">
-        <v>-0.008716198511418954</v>
+        <v>-0.008716199320743427</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.008716198511418954</v>
+        <v>-0.008716199320743427</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.008716198511418954</v>
+        <v>-0.008716199320743427</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.008716198511418954</v>
-      </c>
-      <c r="M35" t="inlineStr"/>
+        <v>-0.01595359957006743</v>
+      </c>
+      <c r="M35" t="n">
+        <v>-0.01595359957006743</v>
+      </c>
       <c r="N35" t="n">
         <v>-0.01595359957006743</v>
       </c>
@@ -2545,16 +2438,9 @@
         <v>-0.01595359957006743</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.01595359957006743</v>
+        <v>11</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.01595359957006743</v>
-      </c>
-      <c r="S35" t="inlineStr"/>
-      <c r="T35" t="n">
-        <v>11</v>
-      </c>
-      <c r="U35" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2565,57 +2451,54 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.03531744155444839</v>
+        <v>0.03531734795465337</v>
       </c>
       <c r="C36" t="n">
-        <v>0.1098545561488556</v>
+        <v>0.1098544558103944</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1403069331125718</v>
+        <v>0.1403067396141508</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1365299151341724</v>
+        <v>0.1365298123840758</v>
       </c>
       <c r="F36" t="n">
-        <v>0.1365299151341724</v>
-      </c>
-      <c r="G36" t="inlineStr"/>
+        <v>0.1365298123840758</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.03531734795465296</v>
+      </c>
       <c r="H36" t="n">
-        <v>0.03531744155444865</v>
+        <v>0.1098544558103944</v>
       </c>
       <c r="I36" t="n">
-        <v>0.1098545561488556</v>
+        <v>0.1403067396141511</v>
       </c>
       <c r="J36" t="n">
-        <v>0.1403069331125718</v>
+        <v>0.1365298123840766</v>
       </c>
       <c r="K36" t="n">
-        <v>0.1365299151341725</v>
+        <v>0.1365298123840766</v>
       </c>
       <c r="L36" t="n">
-        <v>0.1365299151341725</v>
-      </c>
-      <c r="M36" t="inlineStr"/>
+        <v>0.008627026634555536</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.05010940854973507</v>
+      </c>
       <c r="N36" t="n">
-        <v>0.008627026634555536</v>
+        <v>0.088243660481585</v>
       </c>
       <c r="O36" t="n">
-        <v>0.05010940854973507</v>
+        <v>0.08248274553685139</v>
       </c>
       <c r="P36" t="n">
-        <v>0.088243660481585</v>
+        <v>0.08248274553685139</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.08248274553685139</v>
+        <v>96</v>
       </c>
       <c r="R36" t="n">
-        <v>0.08248274553685139</v>
-      </c>
-      <c r="S36" t="inlineStr"/>
-      <c r="T36" t="n">
-        <v>96</v>
-      </c>
-      <c r="U36" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2626,37 +2509,41 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-0.03562891152941184</v>
+        <v>-0.03562890856903323</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.03562891152941184</v>
+        <v>-0.03562890856903323</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.03562891152941184</v>
+        <v>-0.03562890856903323</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.03562891152941184</v>
+        <v>-0.03562890856903323</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.03562891152941184</v>
-      </c>
-      <c r="G37" t="inlineStr"/>
+        <v>-0.03562890856903323</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-0.03562890856903322</v>
+      </c>
       <c r="H37" t="n">
-        <v>-0.03562891152941209</v>
+        <v>-0.03562890856903322</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.03562891152941209</v>
+        <v>-0.03562890856903322</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.03562891152941209</v>
+        <v>-0.03562890856903322</v>
       </c>
       <c r="K37" t="n">
-        <v>-0.03562891152941209</v>
+        <v>-0.03562890856903322</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.03562891152941209</v>
-      </c>
-      <c r="M37" t="inlineStr"/>
+        <v>-0.01033649884607192</v>
+      </c>
+      <c r="M37" t="n">
+        <v>-0.01033649884607192</v>
+      </c>
       <c r="N37" t="n">
         <v>-0.01033649884607192</v>
       </c>
@@ -2667,16 +2554,9 @@
         <v>-0.01033649884607192</v>
       </c>
       <c r="Q37" t="n">
-        <v>-0.01033649884607192</v>
+        <v>9</v>
       </c>
       <c r="R37" t="n">
-        <v>-0.01033649884607192</v>
-      </c>
-      <c r="S37" t="inlineStr"/>
-      <c r="T37" t="n">
-        <v>9</v>
-      </c>
-      <c r="U37" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2687,37 +2567,41 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.01143720205249565</v>
+        <v>-0.01143728725963911</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.01143720205249565</v>
+        <v>-0.01143728725963911</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.01143720205249565</v>
+        <v>-0.01143728725963911</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.01143720205249565</v>
+        <v>-0.01143728725963911</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.01143720205249565</v>
-      </c>
-      <c r="G38" t="inlineStr"/>
+        <v>-0.01143728725963911</v>
+      </c>
+      <c r="G38" t="n">
+        <v>-0.01143728725963931</v>
+      </c>
       <c r="H38" t="n">
-        <v>-0.01143720205249576</v>
+        <v>-0.01143728725963931</v>
       </c>
       <c r="I38" t="n">
-        <v>-0.01143720205249576</v>
+        <v>-0.01143728725963931</v>
       </c>
       <c r="J38" t="n">
-        <v>-0.01143720205249576</v>
+        <v>-0.01143728725963931</v>
       </c>
       <c r="K38" t="n">
-        <v>-0.01143720205249576</v>
+        <v>-0.01143728725963931</v>
       </c>
       <c r="L38" t="n">
-        <v>-0.01143720205249576</v>
-      </c>
-      <c r="M38" t="inlineStr"/>
+        <v>-0.007079029824764999</v>
+      </c>
+      <c r="M38" t="n">
+        <v>-0.007079029824764999</v>
+      </c>
       <c r="N38" t="n">
         <v>-0.007079029824764999</v>
       </c>
@@ -2728,16 +2612,9 @@
         <v>-0.007079029824764999</v>
       </c>
       <c r="Q38" t="n">
-        <v>-0.007079029824764999</v>
+        <v>13</v>
       </c>
       <c r="R38" t="n">
-        <v>-0.007079029824764999</v>
-      </c>
-      <c r="S38" t="inlineStr"/>
-      <c r="T38" t="n">
-        <v>13</v>
-      </c>
-      <c r="U38" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2748,39 +2625,43 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.08401911947960014</v>
+        <v>0.08401902560048664</v>
       </c>
       <c r="C39" t="n">
-        <v>0.09739648515493289</v>
+        <v>0.09739639011730179</v>
       </c>
       <c r="D39" t="n">
-        <v>0.09739648515493289</v>
+        <v>0.09739639011730179</v>
       </c>
       <c r="E39" t="n">
-        <v>0.09739648515493289</v>
+        <v>0.09739639011730179</v>
       </c>
       <c r="F39" t="n">
-        <v>0.09739648515493289</v>
-      </c>
-      <c r="G39" t="inlineStr"/>
+        <v>0.09739639011730179</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.08401902560048681</v>
+      </c>
       <c r="H39" t="n">
-        <v>0.0840191194796</v>
+        <v>0.09739639011730165</v>
       </c>
       <c r="I39" t="n">
-        <v>0.09739648515493236</v>
+        <v>0.09739639011730165</v>
       </c>
       <c r="J39" t="n">
-        <v>0.09739648515493236</v>
+        <v>0.09739639011730165</v>
       </c>
       <c r="K39" t="n">
-        <v>0.09739648515493236</v>
+        <v>0.09739639011730165</v>
       </c>
       <c r="L39" t="n">
-        <v>0.09739648515493236</v>
-      </c>
-      <c r="M39" t="inlineStr"/>
+        <v>0.05421560675249947</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0.09092683298453486</v>
+      </c>
       <c r="N39" t="n">
-        <v>0.05421560675249947</v>
+        <v>0.09092683298453486</v>
       </c>
       <c r="O39" t="n">
         <v>0.09092683298453486</v>
@@ -2789,16 +2670,9 @@
         <v>0.09092683298453486</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.09092683298453486</v>
+        <v>49</v>
       </c>
       <c r="R39" t="n">
-        <v>0.09092683298453486</v>
-      </c>
-      <c r="S39" t="inlineStr"/>
-      <c r="T39" t="n">
-        <v>49</v>
-      </c>
-      <c r="U39" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2823,23 +2697,27 @@
       <c r="F40" t="n">
         <v>-0.03737734263396213</v>
       </c>
-      <c r="G40" t="inlineStr"/>
+      <c r="G40" t="n">
+        <v>-0.0373773426339623</v>
+      </c>
       <c r="H40" t="n">
-        <v>-0.03737734263396229</v>
+        <v>-0.0373773426339623</v>
       </c>
       <c r="I40" t="n">
-        <v>-0.03737734263396229</v>
+        <v>-0.0373773426339623</v>
       </c>
       <c r="J40" t="n">
-        <v>-0.03737734263396229</v>
+        <v>-0.0373773426339623</v>
       </c>
       <c r="K40" t="n">
-        <v>-0.03737734263396229</v>
+        <v>-0.0373773426339623</v>
       </c>
       <c r="L40" t="n">
-        <v>-0.03737734263396229</v>
-      </c>
-      <c r="M40" t="inlineStr"/>
+        <v>0.0012066266401572</v>
+      </c>
+      <c r="M40" t="n">
+        <v>0.0012066266401572</v>
+      </c>
       <c r="N40" t="n">
         <v>0.0012066266401572</v>
       </c>
@@ -2850,16 +2728,9 @@
         <v>0.0012066266401572</v>
       </c>
       <c r="Q40" t="n">
-        <v>0.0012066266401572</v>
+        <v>12</v>
       </c>
       <c r="R40" t="n">
-        <v>0.0012066266401572</v>
-      </c>
-      <c r="S40" t="inlineStr"/>
-      <c r="T40" t="n">
-        <v>12</v>
-      </c>
-      <c r="U40" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2884,23 +2755,27 @@
       <c r="F41" t="n">
         <v>-0.005754695255560561</v>
       </c>
-      <c r="G41" t="inlineStr"/>
+      <c r="G41" t="n">
+        <v>-0.005754695255560612</v>
+      </c>
       <c r="H41" t="n">
-        <v>-0.005754695255560641</v>
+        <v>-0.005754695255560612</v>
       </c>
       <c r="I41" t="n">
-        <v>-0.005754695255560641</v>
+        <v>-0.005754695255560612</v>
       </c>
       <c r="J41" t="n">
-        <v>-0.005754695255560641</v>
+        <v>-0.005754695255560612</v>
       </c>
       <c r="K41" t="n">
-        <v>-0.005754695255560641</v>
+        <v>-0.005754695255560612</v>
       </c>
       <c r="L41" t="n">
-        <v>-0.005754695255560641</v>
-      </c>
-      <c r="M41" t="inlineStr"/>
+        <v>0.0005705832608251727</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.0005705832608251727</v>
+      </c>
       <c r="N41" t="n">
         <v>0.0005705832608251727</v>
       </c>
@@ -2911,24 +2786,17 @@
         <v>0.0005705832608251727</v>
       </c>
       <c r="Q41" t="n">
-        <v>0.0005705832608251727</v>
+        <v>1</v>
       </c>
       <c r="R41" t="n">
-        <v>0.0005705832608251727</v>
-      </c>
-      <c r="S41" t="inlineStr"/>
-      <c r="T41" t="n">
-        <v>1</v>
-      </c>
-      <c r="U41" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>